<commit_message>
issue #5: add portion and total(area*portion) of land
</commit_message>
<xml_diff>
--- a/legislator/property/output/normal/丁守中_2012-04-02_財產申報表_tmpf49e1.xlsx
+++ b/legislator/property/output/normal/丁守中_2012-04-02_財產申報表_tmpf49e1.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="91">
   <si>
     <t>name</t>
   </si>
@@ -65,18 +65,21 @@
     <t>index</t>
   </si>
   <si>
+    <t>portion</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>臺北市北投區振興段一小段00660000地號</t>
+  </si>
+  <si>
     <t>臺北市北投區振興段一小段00930000地號</t>
   </si>
   <si>
-    <t>臺北市北投區振興段一小段00660000地號</t>
-  </si>
-  <si>
     <t>臺北市北投區振興段一小段00210008地號</t>
   </si>
   <si>
-    <t>10000分之101</t>
-  </si>
-  <si>
     <t>97300分之4170</t>
   </si>
   <si>
@@ -95,129 +98,90 @@
     <t>溫子苓</t>
   </si>
   <si>
+    <t>93年08月19日</t>
+  </si>
+  <si>
+    <t>85年05月24日</t>
+  </si>
+  <si>
+    <t>97年07月22日</t>
+  </si>
+  <si>
+    <t>繼承</t>
+  </si>
+  <si>
+    <t>nn貝買</t>
+  </si>
+  <si>
+    <t>買賣</t>
+  </si>
+  <si>
+    <t>(超過五年）</t>
+  </si>
+  <si>
+    <t>(超渦年)</t>
+  </si>
+  <si>
+    <t>land</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>2012-04-02</t>
+  </si>
+  <si>
+    <t>tmpf49e1</t>
+  </si>
+  <si>
+    <t>臺北市北投區振興段一小段12407000建號</t>
+  </si>
+  <si>
+    <t>78年10月11B</t>
+  </si>
+  <si>
+    <t>臺北市北投區振興段一小段12496000建號</t>
+  </si>
+  <si>
+    <t>臺北市北投區振興段一小段12398000建號</t>
+  </si>
+  <si>
+    <t>臺北市北投區振興段一小段12884000建號</t>
+  </si>
+  <si>
+    <t>臺北市北投區振興段一小段12891000建號</t>
+  </si>
+  <si>
+    <t>56分之1</t>
+  </si>
+  <si>
+    <t>100000分之4464</t>
+  </si>
+  <si>
+    <t>r守中</t>
+  </si>
+  <si>
     <t>78年10月11曰</t>
   </si>
   <si>
-    <t>93年08月19日</t>
-  </si>
-  <si>
-    <t>85年05月24日</t>
-  </si>
-  <si>
-    <t>97年07月22日</t>
-  </si>
-  <si>
-    <t>買賣</t>
-  </si>
-  <si>
-    <t>繼承</t>
-  </si>
-  <si>
-    <t>nn貝買</t>
-  </si>
-  <si>
-    <t>(超過五年）</t>
-  </si>
-  <si>
-    <t>(超渦年)</t>
-  </si>
-  <si>
-    <t>land</t>
-  </si>
-  <si>
-    <t>normal</t>
-  </si>
-  <si>
-    <t>2012-04-02</t>
-  </si>
-  <si>
-    <t>tmpf49e1</t>
-  </si>
-  <si>
-    <t>建物標示</t>
-  </si>
-  <si>
-    <t>面積（平方公尺）</t>
-  </si>
-  <si>
-    <t>權利範圍(持分）</t>
-  </si>
-  <si>
-    <t>所有權人</t>
-  </si>
-  <si>
-    <t>登記（取得）時間</t>
-  </si>
-  <si>
-    <t>登記（取得）原因</t>
-  </si>
-  <si>
-    <t>取得價額</t>
-  </si>
-  <si>
-    <t>臺北市北投區振興段一小段12407000建號</t>
-  </si>
-  <si>
-    <t>臺北市北投區振興段一小段12496000建號</t>
-  </si>
-  <si>
-    <t>臺北市北投區振興段一小段12398000建號</t>
-  </si>
-  <si>
-    <t>臺北市北投區振興段一小段12884000建號</t>
-  </si>
-  <si>
-    <t>臺北市北投區振興段一小段12891000建號</t>
-  </si>
-  <si>
-    <t>56分之1</t>
-  </si>
-  <si>
-    <t>100000分之4464</t>
-  </si>
-  <si>
-    <t>r守中</t>
-  </si>
-  <si>
-    <t>78年10月11B</t>
-  </si>
-  <si>
     <t>(超堝石年)</t>
   </si>
   <si>
-    <t>廠牌型號</t>
-  </si>
-  <si>
-    <t>汽缸容量</t>
-  </si>
-  <si>
-    <t>所有人</t>
-  </si>
-  <si>
     <t>LEXUSES350(客車）</t>
   </si>
   <si>
     <t>100年04月19闩</t>
   </si>
   <si>
-    <t>存放機構(應敘明分支機構）</t>
-  </si>
-  <si>
-    <t>種類</t>
-  </si>
-  <si>
-    <t>幣別</t>
-  </si>
-  <si>
-    <t>外幣總額</t>
-  </si>
-  <si>
-    <t>新臺幣總額或折合新臺幣總額</t>
-  </si>
-  <si>
     <t>台北富邦商業銀行</t>
   </si>
   <si>
+    <t>活期儲蓄存款</t>
+  </si>
+  <si>
+    <t>新臺幣</t>
+  </si>
+  <si>
     <t>中華郵政股份有限公司</t>
   </si>
   <si>
@@ -239,9 +203,6 @@
     <t>華南商業銀行</t>
   </si>
   <si>
-    <t>活期儲蓄存款</t>
-  </si>
-  <si>
     <t>活期存款</t>
   </si>
   <si>
@@ -251,9 +212,6 @@
     <t>支票存款</t>
   </si>
   <si>
-    <t>新臺幣</t>
-  </si>
-  <si>
     <t>美金</t>
   </si>
   <si>
@@ -266,12 +224,6 @@
     <t>currency</t>
   </si>
   <si>
-    <t>total</t>
-  </si>
-  <si>
-    <t>琉園股份有限公司</t>
-  </si>
-  <si>
     <t>愛樂電台股份有限公司</t>
   </si>
   <si>
@@ -302,15 +254,6 @@
     <t>stock</t>
   </si>
   <si>
-    <t>財產種類</t>
-  </si>
-  <si>
-    <t>項件</t>
-  </si>
-  <si>
-    <t>價額</t>
-  </si>
-  <si>
     <t>手錶</t>
   </si>
   <si>
@@ -320,30 +263,18 @@
     <t>2000000</t>
   </si>
   <si>
-    <t>保險公司</t>
-  </si>
-  <si>
-    <t>保險名稱</t>
-  </si>
-  <si>
-    <t>要保人</t>
-  </si>
-  <si>
-    <t>備註</t>
-  </si>
-  <si>
     <t>南山人壽</t>
   </si>
   <si>
     <t>南山康福20年期終身壽險</t>
   </si>
   <si>
+    <t>20年期年繳68310元</t>
+  </si>
+  <si>
     <t>終身壽險</t>
   </si>
   <si>
-    <t>20年期年繳68310元</t>
-  </si>
-  <si>
     <t>20年期年繳56167元</t>
   </si>
   <si>
@@ -351,24 +282,6 @@
   </si>
   <si>
     <t>新20年期增值分紅年繳41542元</t>
-  </si>
-  <si>
-    <t>(十二）事業投資（總金額：新臺幣990000元）投資人</t>
-  </si>
-  <si>
-    <t>投資事業名稱</t>
-  </si>
-  <si>
-    <t>投資事業地址</t>
-  </si>
-  <si>
-    <t>投資金額</t>
-  </si>
-  <si>
-    <t>取得（發生）時間</t>
-  </si>
-  <si>
-    <t>取得（發生）原因</t>
   </si>
   <si>
     <t>鼎天股份有限公司</t>
@@ -739,13 +652,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:17">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -788,25 +701,31 @@
       <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2">
-        <v>3971</v>
+        <v>973</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>28</v>
@@ -824,7 +743,7 @@
         <v>35</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M2" s="2">
         <v>515</v>
@@ -833,33 +752,39 @@
         <v>36</v>
       </c>
       <c r="O2" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+        <v>14</v>
+      </c>
+      <c r="P2" s="2">
+        <v>0.0428571428571429</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>41.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2">
-        <v>973</v>
+        <v>3971</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>29</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>33</v>
@@ -871,7 +796,7 @@
         <v>35</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M3" s="2">
         <v>515</v>
@@ -880,33 +805,39 @@
         <v>36</v>
       </c>
       <c r="O3" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+        <v>15</v>
+      </c>
+      <c r="P3" s="2">
+        <v>0.0084</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>33.3564</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2">
-        <v>3971</v>
+        <v>2975.21</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>32</v>
+      <c r="H4" s="2">
+        <v>29700000</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>33</v>
@@ -918,7 +849,7 @@
         <v>35</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M4" s="2">
         <v>515</v>
@@ -927,54 +858,13 @@
         <v>36</v>
       </c>
       <c r="O4" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="1">
         <v>16</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="P4" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="2">
         <v>2975.21</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="2">
-        <v>29700000</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M5" s="2">
-        <v>515</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O5" s="2">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -984,7 +874,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -994,46 +884,46 @@
       <c r="B1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="1">
+        <v>193.66</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C2" s="2">
-        <v>193.66</v>
+        <v>2357.46</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>31</v>
@@ -1041,25 +931,25 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C3" s="2">
-        <v>2357.46</v>
+        <v>153.32</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>31</v>
@@ -1067,25 +957,25 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C4" s="2">
-        <v>153.32</v>
+        <v>2357.46</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>31</v>
@@ -1093,22 +983,22 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C5" s="2">
-        <v>2357.46</v>
+        <v>126.18</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>28</v>
@@ -1119,54 +1009,28 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C6" s="2">
-        <v>126.18</v>
+        <v>1350.27</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="1">
-        <v>26</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1350.27</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1176,7 +1040,40 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="B1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="2:7">
+      <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="1">
+        <v>3456</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="1">
+        <v>600000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1184,352 +1081,273 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>43</v>
+        <v>22</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1">
+        <v>139682</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="2">
-        <v>3456</v>
+        <v>53</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="2">
-        <v>600000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="B1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1">
-        <v>51</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2">
-        <v>139682</v>
+        <v>244911</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2">
-        <v>244911</v>
+        <v>664256</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2">
-        <v>664256</v>
+        <v>1915713</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2">
-        <v>1915713</v>
+        <v>149924</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="F6" s="2">
+        <v>10471.02</v>
+      </c>
       <c r="G6" s="2">
-        <v>149924</v>
+        <v>305126</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="2">
-        <v>10471.02</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="F7" s="2"/>
       <c r="G7" s="2">
-        <v>305126</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2">
-        <v>10000</v>
+        <v>733</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2">
-        <v>733</v>
+        <v>55130</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2">
-        <v>55130</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2">
-        <v>5000</v>
+        <v>794873</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2">
-        <v>794873</v>
+        <v>75867</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2">
-        <v>75867</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="1">
-        <v>63</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2">
         <v>194103</v>
       </c>
     </row>
@@ -1540,7 +1358,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1554,16 +1372,16 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>81</v>
+        <v>15</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
@@ -1589,28 +1407,28 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="1">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2">
-        <v>1644599</v>
+        <v>70000</v>
       </c>
       <c r="E2" s="2">
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="2">
+        <v>700000</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="G2" s="2">
-        <v>16445990</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>34</v>
@@ -1619,7 +1437,7 @@
         <v>35</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L2" s="2">
         <v>515</v>
@@ -1628,33 +1446,33 @@
         <v>36</v>
       </c>
       <c r="N2" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="1">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>67</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3" s="2">
-        <v>70000</v>
+        <v>50000</v>
       </c>
       <c r="E3" s="2">
         <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="2">
+        <v>500000</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="G3" s="2">
-        <v>700000</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>34</v>
@@ -1663,7 +1481,7 @@
         <v>35</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L3" s="2">
         <v>515</v>
@@ -1672,33 +1490,33 @@
         <v>36</v>
       </c>
       <c r="N3" s="2">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2">
-        <v>50000</v>
+        <v>240000</v>
       </c>
       <c r="E4" s="2">
         <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2400000</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="G4" s="2">
-        <v>500000</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>34</v>
@@ -1707,7 +1525,7 @@
         <v>35</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L4" s="2">
         <v>515</v>
@@ -1716,33 +1534,33 @@
         <v>36</v>
       </c>
       <c r="N4" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="D5" s="2">
-        <v>240000</v>
+        <v>31274</v>
       </c>
       <c r="E5" s="2">
         <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="2">
+        <v>312740</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="G5" s="2">
-        <v>2400000</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>34</v>
@@ -1751,7 +1569,7 @@
         <v>35</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L5" s="2">
         <v>515</v>
@@ -1760,33 +1578,33 @@
         <v>36</v>
       </c>
       <c r="N5" s="2">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="D6" s="2">
-        <v>31274</v>
+        <v>250000</v>
       </c>
       <c r="E6" s="2">
         <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="G6" s="2">
-        <v>312740</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>34</v>
@@ -1795,7 +1613,7 @@
         <v>35</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L6" s="2">
         <v>515</v>
@@ -1804,33 +1622,33 @@
         <v>36</v>
       </c>
       <c r="N6" s="2">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="2">
-        <v>250000</v>
+        <v>200000</v>
       </c>
       <c r="E7" s="2">
         <v>10</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2000000</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>34</v>
@@ -1839,7 +1657,7 @@
         <v>35</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L7" s="2">
         <v>515</v>
@@ -1848,33 +1666,33 @@
         <v>36</v>
       </c>
       <c r="N7" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="1">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D8" s="2">
-        <v>200000</v>
+        <v>115000</v>
       </c>
       <c r="E8" s="2">
         <v>10</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1150000</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="G8" s="2">
-        <v>2000000</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>34</v>
@@ -1883,7 +1701,7 @@
         <v>35</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L8" s="2">
         <v>515</v>
@@ -1892,33 +1710,33 @@
         <v>36</v>
       </c>
       <c r="N8" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D9" s="2">
-        <v>115000</v>
+        <v>40000</v>
       </c>
       <c r="E9" s="2">
         <v>10</v>
       </c>
       <c r="F9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="2">
+        <v>400000</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="G9" s="2">
-        <v>1150000</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>34</v>
@@ -1927,7 +1745,7 @@
         <v>35</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L9" s="2">
         <v>515</v>
@@ -1936,33 +1754,33 @@
         <v>36</v>
       </c>
       <c r="N9" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="1">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D10" s="2">
-        <v>40000</v>
+        <v>48000</v>
       </c>
       <c r="E10" s="2">
         <v>10</v>
       </c>
       <c r="F10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="2">
+        <v>480000</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="G10" s="2">
-        <v>400000</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>34</v>
@@ -1971,7 +1789,7 @@
         <v>35</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L10" s="2">
         <v>515</v>
@@ -1980,50 +1798,6 @@
         <v>36</v>
       </c>
       <c r="N10" s="2">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="1">
-        <v>80</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="2">
-        <v>48000</v>
-      </c>
-      <c r="E11" s="2">
-        <v>10</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G11" s="2">
-        <v>480000</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L11" s="2">
-        <v>515</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N11" s="2">
         <v>80</v>
       </c>
     </row>
@@ -2034,7 +1808,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2042,50 +1816,33 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>94</v>
+        <v>77</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>95</v>
+        <v>22</v>
+      </c>
+      <c r="E1" s="1">
+        <v>600000</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="C2" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="2">
-        <v>600000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1">
-        <v>100</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C3" s="2">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>98</v>
+        <v>24</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2095,7 +1852,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2103,84 +1860,67 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>101</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1">
-        <v>108</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2190,53 +1930,30 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="B1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="2:7">
       <c r="B1" s="1" t="s">
-        <v>110</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>113</v>
+        <v>88</v>
+      </c>
+      <c r="E1" s="1">
+        <v>990000</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1">
-        <v>123</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E2" s="2">
-        <v>990000</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#5: property building done
</commit_message>
<xml_diff>
--- a/legislator/property/output/normal/丁守中_2012-04-02_財產申報表_tmpf49e1.xlsx
+++ b/legislator/property/output/normal/丁守中_2012-04-02_財產申報表_tmpf49e1.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="93">
   <si>
     <t>name</t>
   </si>
@@ -71,15 +71,18 @@
     <t>total</t>
   </si>
   <si>
+    <t>臺北市北投區振興段一小段00930000地號</t>
+  </si>
+  <si>
     <t>臺北市北投區振興段一小段00660000地號</t>
   </si>
   <si>
-    <t>臺北市北投區振興段一小段00930000地號</t>
-  </si>
-  <si>
     <t>臺北市北投區振興段一小段00210008地號</t>
   </si>
   <si>
+    <t>10000分之101</t>
+  </si>
+  <si>
     <t>97300分之4170</t>
   </si>
   <si>
@@ -98,6 +101,9 @@
     <t>溫子苓</t>
   </si>
   <si>
+    <t>78年10月11曰</t>
+  </si>
+  <si>
     <t>93年08月19日</t>
   </si>
   <si>
@@ -107,15 +113,15 @@
     <t>97年07月22日</t>
   </si>
   <si>
+    <t>買賣</t>
+  </si>
+  <si>
     <t>繼承</t>
   </si>
   <si>
     <t>nn貝買</t>
   </si>
   <si>
-    <t>買賣</t>
-  </si>
-  <si>
     <t>(超過五年）</t>
   </si>
   <si>
@@ -137,33 +143,30 @@
     <t>臺北市北投區振興段一小段12407000建號</t>
   </si>
   <si>
+    <t>臺北市北投區振興段一小段12496000建號</t>
+  </si>
+  <si>
+    <t>臺北市北投區振興段一小段12398000建號</t>
+  </si>
+  <si>
+    <t>臺北市北投區振興段一小段12884000建號</t>
+  </si>
+  <si>
+    <t>臺北市北投區振興段一小段12891000建號</t>
+  </si>
+  <si>
+    <t>56分之1</t>
+  </si>
+  <si>
+    <t>100000分之4464</t>
+  </si>
+  <si>
+    <t>r守中</t>
+  </si>
+  <si>
     <t>78年10月11B</t>
   </si>
   <si>
-    <t>臺北市北投區振興段一小段12496000建號</t>
-  </si>
-  <si>
-    <t>臺北市北投區振興段一小段12398000建號</t>
-  </si>
-  <si>
-    <t>臺北市北投區振興段一小段12884000建號</t>
-  </si>
-  <si>
-    <t>臺北市北投區振興段一小段12891000建號</t>
-  </si>
-  <si>
-    <t>56分之1</t>
-  </si>
-  <si>
-    <t>100000分之4464</t>
-  </si>
-  <si>
-    <t>r守中</t>
-  </si>
-  <si>
-    <t>78年10月11曰</t>
-  </si>
-  <si>
     <t>(超堝石年)</t>
   </si>
   <si>
@@ -222,6 +225,9 @@
   </si>
   <si>
     <t>currency</t>
+  </si>
+  <si>
+    <t>琉園股份有限公司</t>
   </si>
   <si>
     <t>愛樂電台股份有限公司</t>
@@ -652,7 +658,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -710,66 +716,66 @@
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="2">
-        <v>973</v>
+        <v>3971</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M2" s="2">
         <v>515</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="O2" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P2" s="2">
-        <v>0.0428571428571429</v>
+        <v>0.0101</v>
       </c>
       <c r="Q2" s="2">
-        <v>41.7</v>
+        <v>40.1071</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="2">
-        <v>3971</v>
+        <v>973</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>20</v>
@@ -778,51 +784,51 @@
         <v>23</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M3" s="2">
         <v>515</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="O3" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P3" s="2">
-        <v>0.0084</v>
+        <v>0.0428571428571429</v>
       </c>
       <c r="Q3" s="2">
-        <v>33.3564</v>
+        <v>41.7</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="1">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="C4" s="2">
-        <v>2975.21</v>
+        <v>3971</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>21</v>
@@ -831,39 +837,92 @@
         <v>24</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="2">
-        <v>29700000</v>
+        <v>32</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M4" s="2">
         <v>515</v>
       </c>
       <c r="N4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O4" s="2">
+        <v>15</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0.0084</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>33.3564</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="1">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2975.21</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="2">
+        <v>29700000</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="O4" s="2">
+      <c r="K5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="2">
+        <v>515</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" s="2">
         <v>16</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P5" s="2">
         <v>1</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="Q5" s="2">
         <v>2975.21</v>
       </c>
     </row>
@@ -874,76 +933,130 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:17">
       <c r="B1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="1">
-        <v>193.66</v>
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="1">
         <v>21</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1">
-        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C2" s="2">
-        <v>2357.46</v>
+        <v>193.66</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>33</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="2">
+        <v>515</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O2" s="2">
+        <v>21</v>
+      </c>
+      <c r="P2" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>193.66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C3" s="2">
-        <v>153.32</v>
+        <v>2357.46</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>26</v>
@@ -952,85 +1065,246 @@
         <v>30</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>33</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="2">
+        <v>515</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="2">
+        <v>22</v>
+      </c>
+      <c r="P3" s="2">
+        <v>0.0178571428571429</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>42.0975</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C4" s="2">
-        <v>2357.46</v>
+        <v>153.32</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>33</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="2">
+        <v>515</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O4" s="2">
+        <v>23</v>
+      </c>
+      <c r="P4" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>153.32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="2">
-        <v>126.18</v>
+        <v>2357.46</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>33</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="2">
+        <v>515</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" s="2">
+        <v>24</v>
+      </c>
+      <c r="P5" s="2">
+        <v>0.0178571428571429</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>42.0975</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C6" s="2">
+        <v>126.18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" s="2">
+        <v>515</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O6" s="2">
+        <v>25</v>
+      </c>
+      <c r="P6" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>126.18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="1">
+        <v>26</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="2">
         <v>1350.27</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>47</v>
+      <c r="D7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" s="2">
+        <v>515</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O7" s="2">
+        <v>26</v>
+      </c>
+      <c r="P7" s="2">
+        <v>0.04464</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>60.2760528</v>
       </c>
     </row>
   </sheetData>
@@ -1040,29 +1314,52 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:7">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1">
         <v>3456</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>30</v>
       </c>
       <c r="G1" s="1">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1">
+        <v>36</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="2">
+        <v>3456</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="2">
         <v>600000</v>
       </c>
     </row>
@@ -1073,7 +1370,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1081,16 +1378,16 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1">
@@ -1099,255 +1396,276 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1">
+        <v>51</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2">
-        <v>244911</v>
+        <v>139682</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2">
-        <v>664256</v>
+        <v>244911</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2">
-        <v>1915713</v>
+        <v>664256</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2">
-        <v>149924</v>
+        <v>1915713</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="2">
-        <v>10471.02</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F6" s="2"/>
       <c r="G6" s="2">
-        <v>305126</v>
+        <v>149924</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>62</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="F7" s="2">
+        <v>10471.02</v>
+      </c>
       <c r="G7" s="2">
-        <v>10000</v>
+        <v>305126</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2">
-        <v>733</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2">
-        <v>55130</v>
+        <v>733</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2">
-        <v>5000</v>
+        <v>55130</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2">
-        <v>794873</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2">
-        <v>75867</v>
+        <v>794873</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2">
+        <v>75867</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="1">
+        <v>63</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2">
         <v>194103</v>
       </c>
     </row>
@@ -1358,7 +1676,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1372,13 +1690,13 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>15</v>
@@ -1407,397 +1725,441 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="1">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2">
-        <v>70000</v>
+        <v>1644599</v>
       </c>
       <c r="E2" s="2">
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G2" s="2">
-        <v>700000</v>
+        <v>16445990</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L2" s="2">
         <v>515</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N2" s="2">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="1">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D3" s="2">
-        <v>50000</v>
+        <v>70000</v>
       </c>
       <c r="E3" s="2">
         <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G3" s="2">
-        <v>500000</v>
+        <v>700000</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L3" s="2">
         <v>515</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N3" s="2">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2">
-        <v>240000</v>
+        <v>50000</v>
       </c>
       <c r="E4" s="2">
         <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G4" s="2">
-        <v>2400000</v>
+        <v>500000</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L4" s="2">
         <v>515</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N4" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>74</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2">
-        <v>31274</v>
+        <v>240000</v>
       </c>
       <c r="E5" s="2">
         <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G5" s="2">
-        <v>312740</v>
+        <v>2400000</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L5" s="2">
         <v>515</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N5" s="2">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1">
+        <v>75</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="D6" s="2">
-        <v>250000</v>
+        <v>31274</v>
       </c>
       <c r="E6" s="2">
         <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>75</v>
+        <v>53</v>
+      </c>
+      <c r="G6" s="2">
+        <v>312740</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L6" s="2">
         <v>515</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N6" s="2">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D7" s="2">
-        <v>200000</v>
+        <v>250000</v>
       </c>
       <c r="E7" s="2">
         <v>10</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" s="2">
-        <v>2000000</v>
+        <v>53</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L7" s="2">
         <v>515</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N7" s="2">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="1">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2">
-        <v>115000</v>
+        <v>200000</v>
       </c>
       <c r="E8" s="2">
         <v>10</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G8" s="2">
-        <v>1150000</v>
+        <v>2000000</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L8" s="2">
         <v>515</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N8" s="2">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" s="2">
-        <v>40000</v>
+        <v>115000</v>
       </c>
       <c r="E9" s="2">
         <v>10</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G9" s="2">
-        <v>400000</v>
+        <v>1150000</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L9" s="2">
         <v>515</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N9" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="1">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D10" s="2">
-        <v>48000</v>
+        <v>40000</v>
       </c>
       <c r="E10" s="2">
         <v>10</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G10" s="2">
-        <v>480000</v>
+        <v>400000</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L10" s="2">
         <v>515</v>
       </c>
       <c r="M10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N10" s="2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="1">
+        <v>80</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="2">
+        <v>48000</v>
+      </c>
+      <c r="E11" s="2">
+        <v>10</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="2">
+        <v>480000</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="N10" s="2">
+      <c r="J11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" s="2">
+        <v>515</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N11" s="2">
         <v>80</v>
       </c>
     </row>
@@ -1808,7 +2170,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1816,13 +2178,13 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C1" s="1">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1">
         <v>600000</v>
@@ -1830,19 +2192,36 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1">
+        <v>99</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="2">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
         <v>100</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="2">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>79</v>
+      <c r="D3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1852,7 +2231,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1860,30 +2239,30 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>84</v>
@@ -1891,36 +2270,53 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>83</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1">
+        <v>107</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1">
         <v>108</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>86</v>
+      <c r="B5" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1930,30 +2326,53 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:7">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1">
         <v>990000</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1">
+        <v>123</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>90</v>
+      </c>
+      <c r="E2" s="2">
+        <v>990000</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix some dirty files
</commit_message>
<xml_diff>
--- a/legislator/property/output/normal/丁守中_2012-04-02_財產申報表_tmpf49e1.xlsx
+++ b/legislator/property/output/normal/丁守中_2012-04-02_財產申報表_tmpf49e1.xlsx
@@ -15,13 +15,14 @@
     <sheet name="具有相當價值之財產" sheetId="6" r:id="rId6"/>
     <sheet name="保險" sheetId="7" r:id="rId7"/>
     <sheet name="債務" sheetId="8" r:id="rId8"/>
+    <sheet name="事業投資" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="107">
   <si>
     <t>name</t>
   </si>
@@ -311,6 +312,24 @@
     <t>debtor</t>
   </si>
   <si>
+    <t>房岸十地抵押貸款</t>
+  </si>
+  <si>
+    <t>華南商業銀行臺北市北投區北投路</t>
+  </si>
+  <si>
+    <t>100年01月10日</t>
+  </si>
+  <si>
+    <t>房屋土地抵押貸款</t>
+  </si>
+  <si>
+    <t>debt</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
     <t>鼎天股份有限公司</t>
   </si>
   <si>
@@ -323,7 +342,7 @@
     <t>投資</t>
   </si>
   <si>
-    <t>debt</t>
+    <t>investment</t>
   </si>
 </sst>
 </file>
@@ -2823,6 +2842,148 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="B1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="1">
+        <v>120</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" s="2">
+        <v>15757122</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="2">
+        <v>515</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" s="2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="1">
+        <v>121</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" s="2">
+        <v>9510466</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="2">
+        <v>515</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" s="2">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2831,13 +2992,13 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="B1" s="1" t="s">
-        <v>94</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>101</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>15</v>
@@ -2872,28 +3033,28 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="1">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="E2" s="2">
         <v>990000</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>36</v>
@@ -2911,7 +3072,7 @@
         <v>38</v>
       </c>
       <c r="N2" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>